<commit_message>
implementar validacao de dados no bd nas pipelines
</commit_message>
<xml_diff>
--- a/dashboards_melhorados/sessoes_ia_completas.xlsx
+++ b/dashboards_melhorados/sessoes_ia_completas.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -528,7 +528,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Anômala</t>
+          <t>Normal</t>
         </is>
       </c>
     </row>
@@ -713,6 +713,99 @@
         <v>1</v>
       </c>
       <c r="G9" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>aline</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>aline@gmail.com</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>06/06/2025</t>
+        </is>
+      </c>
+      <c r="E10" t="n">
+        <v>70.25</v>
+      </c>
+      <c r="F10" t="n">
+        <v>4</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Anômala</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>vih</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>vih@gmail.com</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>06/06/2025</t>
+        </is>
+      </c>
+      <c r="E11" t="n">
+        <v>8.983333333333333</v>
+      </c>
+      <c r="F11" t="n">
+        <v>4</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Normal</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>cad</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>cad@gmail.com</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>06/06/2025</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>0.2833333333333333</v>
+      </c>
+      <c r="F12" t="n">
+        <v>3</v>
+      </c>
+      <c r="G12" t="inlineStr">
         <is>
           <t>Normal</t>
         </is>

</xml_diff>